<commit_message>
Update default row number.
</commit_message>
<xml_diff>
--- a/app-dev/_resources/default_krbiz_order_unified_row_names.xlsx
+++ b/app-dev/_resources/default_krbiz_order_unified_row_names.xlsx
@@ -240,7 +240,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +251,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -293,10 +299,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -728,7 +734,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -774,7 +780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -816,12 +822,12 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>17</v>
@@ -858,7 +864,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -902,7 +908,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
@@ -944,7 +950,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="1" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Update the sheet name.
</commit_message>
<xml_diff>
--- a/app-dev/_resources/default_krbiz_order_unified_row_names.xlsx
+++ b/app-dev/_resources/default_krbiz_order_unified_row_names.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0" firstSheet="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1" state="visible"/>
+    <sheet name="variable_mapping" sheetId="1" r:id="rId1" state="visible"/>
   </sheets>
 </workbook>
 </file>
@@ -509,22 +509,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.17" customWidth="1"/>
-    <col min="2" max="2" width="14.79" customWidth="1"/>
-    <col min="3" max="3" width="13.33" customWidth="1"/>
-    <col min="4" max="4" width="19.17" customWidth="1"/>
-    <col min="5" max="5" width="17.71" customWidth="1"/>
-    <col min="6" max="6" width="26.46" customWidth="1"/>
-    <col min="7" max="7" width="22.08" customWidth="1"/>
-    <col min="8" max="8" width="25.00" customWidth="1"/>
-    <col min="9" max="9" width="17.71" customWidth="1"/>
-    <col min="10" max="10" width="19.17" customWidth="1"/>
-    <col min="11" max="11" width="27.92" customWidth="1"/>
-    <col min="12" max="12" width="20.63" customWidth="1"/>
-    <col min="13" max="13" width="36.67" customWidth="1"/>
-    <col min="14" max="14" width="20.63" customWidth="1"/>
-    <col min="15" max="15" width="13.33" customWidth="1"/>
-    <col min="16" max="16" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="14.48" customWidth="1"/>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.21" customWidth="1"/>
+    <col min="4" max="4" width="14.48" customWidth="1"/>
+    <col min="5" max="5" width="13.33" customWidth="1"/>
+    <col min="6" max="6" width="19.79" customWidth="1"/>
+    <col min="7" max="7" width="16.56" customWidth="1"/>
+    <col min="8" max="8" width="18.75" customWidth="1"/>
+    <col min="9" max="9" width="13.33" customWidth="1"/>
+    <col min="10" max="10" width="14.48" customWidth="1"/>
+    <col min="11" max="11" width="20.83" customWidth="1"/>
+    <col min="12" max="12" width="15.52" customWidth="1"/>
+    <col min="13" max="13" width="27.19" customWidth="1"/>
+    <col min="14" max="14" width="15.52" customWidth="1"/>
+    <col min="15" max="15" width="10.21" customWidth="1"/>
+    <col min="16" max="16" width="12.29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>